<commit_message>
added Location on results; changed XY degrees to Lat Long
</commit_message>
<xml_diff>
--- a/ProgramSrc/ReportTemplate.xlsx
+++ b/ProgramSrc/ReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\ProgramSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCE291B-C916-421C-884F-F7274F2B73AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F588A91-7B94-4F5E-8408-7BE2DA9C4039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{EDF13D95-9A8A-4EF7-9253-EE93AC25A225}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EDF13D95-9A8A-4EF7-9253-EE93AC25A225}"/>
   </bookViews>
   <sheets>
     <sheet name="Shelter Location-Allocation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Shelter Location - Allocation  Report</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Shelter Assigned</t>
   </si>
   <si>
-    <t>Shelter Level</t>
-  </si>
-  <si>
     <t>Using Bilevel No Transfer (BNT) Model</t>
   </si>
   <si>
@@ -109,13 +106,28 @@
   </si>
   <si>
     <t>MaxDistance</t>
+  </si>
+  <si>
+    <t>Commmunity Longitude</t>
+  </si>
+  <si>
+    <t>Commmunity Latitude</t>
+  </si>
+  <si>
+    <t>Shelter Longitude</t>
+  </si>
+  <si>
+    <t>Shelter Latitude</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +147,12 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -589,13 +607,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color theme="9" tint="-0.499984740745262"/>
         </top>
@@ -627,6 +638,13 @@
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -719,20 +737,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5C4CC10-88FC-4A5B-8C71-99243C0E26D1}" name="Table2" displayName="Table2" ref="A4:D55" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13">
-  <autoFilter ref="A4:D55" xr:uid="{A5C4CC10-88FC-4A5B-8C71-99243C0E26D1}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5C4CC10-88FC-4A5B-8C71-99243C0E26D1}" name="Table2" displayName="Table2" ref="A4:H55" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13">
+  <autoFilter ref="A4:H55" xr:uid="{A5C4CC10-88FC-4A5B-8C71-99243C0E26D1}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D3DEF85D-7FCB-4172-8B8D-A02B23888F24}" name="Community"/>
     <tableColumn id="2" xr3:uid="{3BE21453-8549-460B-92A8-0EDB474BDA35}" name="Allocated Individuals"/>
-    <tableColumn id="3" xr3:uid="{F8522F93-374E-4958-921D-67AE8F804243}" name="Shelter Assigned"/>
-    <tableColumn id="4" xr3:uid="{A61A7FB6-17E1-4928-BA0D-035C323612F7}" name="Shelter Level"/>
+    <tableColumn id="3" xr3:uid="{F8522F93-374E-4958-921D-67AE8F804243}" name="Commmunity Longitude"/>
+    <tableColumn id="4" xr3:uid="{A61A7FB6-17E1-4928-BA0D-035C323612F7}" name="Commmunity Latitude"/>
+    <tableColumn id="5" xr3:uid="{91027B5D-1918-4F9D-BB6E-69B038899538}" name="Shelter Assigned"/>
+    <tableColumn id="6" xr3:uid="{69D03C93-59D0-46C6-998E-A931A82399AC}" name="Level"/>
+    <tableColumn id="7" xr3:uid="{38234185-885C-417C-BEC6-8B0AAC5BC3AF}" name="Shelter Longitude"/>
+    <tableColumn id="8" xr3:uid="{2914792C-C302-4F22-9934-AAC0281D3D53}" name="Shelter Latitude"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B4ED4F0-0F30-4D83-A605-68AD3ECCA052}" name="Table62" displayName="Table62" ref="A1:H50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B4ED4F0-0F30-4D83-A605-68AD3ECCA052}" name="Table62" displayName="Table62" ref="A1:H50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H50" xr:uid="{2B4ED4F0-0F30-4D83-A605-68AD3ECCA052}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1098318C-F159-4C06-B902-D5D443D7C297}" name="Active" dataDxfId="7"/>
@@ -1067,64 +1089,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A918FFA0-D07D-44CC-B35F-E2BA18996B1D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="3" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="8" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1147,7 +1196,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1174,28 +1223,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1700,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F6E060-A238-4890-9731-8C688E2E947F}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
@@ -1716,43 +1765,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report previewing; Password  input dynamic
</commit_message>
<xml_diff>
--- a/ProgramSrc/ReportTemplate.xlsx
+++ b/ProgramSrc/ReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\ProgramSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F588A91-7B94-4F5E-8408-7BE2DA9C4039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D2987-C7F1-457D-A7A2-062BA3E6AFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EDF13D95-9A8A-4EF7-9253-EE93AC25A225}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>Allocated Individuals</t>
-  </si>
-  <si>
     <t>Shelter Assigned</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Allocated Population</t>
   </si>
 </sst>
 </file>
@@ -267,11 +267,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,13 +741,13 @@
   <autoFilter ref="A4:H55" xr:uid="{A5C4CC10-88FC-4A5B-8C71-99243C0E26D1}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D3DEF85D-7FCB-4172-8B8D-A02B23888F24}" name="Community"/>
-    <tableColumn id="2" xr3:uid="{3BE21453-8549-460B-92A8-0EDB474BDA35}" name="Allocated Individuals"/>
-    <tableColumn id="3" xr3:uid="{F8522F93-374E-4958-921D-67AE8F804243}" name="Commmunity Longitude"/>
-    <tableColumn id="4" xr3:uid="{A61A7FB6-17E1-4928-BA0D-035C323612F7}" name="Commmunity Latitude"/>
+    <tableColumn id="2" xr3:uid="{3BE21453-8549-460B-92A8-0EDB474BDA35}" name="Allocated Population"/>
+    <tableColumn id="3" xr3:uid="{F8522F93-374E-4958-921D-67AE8F804243}" name="Commmunity Latitude"/>
+    <tableColumn id="4" xr3:uid="{A61A7FB6-17E1-4928-BA0D-035C323612F7}" name="Commmunity Longitude"/>
     <tableColumn id="5" xr3:uid="{91027B5D-1918-4F9D-BB6E-69B038899538}" name="Shelter Assigned"/>
     <tableColumn id="6" xr3:uid="{69D03C93-59D0-46C6-998E-A931A82399AC}" name="Level"/>
-    <tableColumn id="7" xr3:uid="{38234185-885C-417C-BEC6-8B0AAC5BC3AF}" name="Shelter Longitude"/>
-    <tableColumn id="8" xr3:uid="{2914792C-C302-4F22-9934-AAC0281D3D53}" name="Shelter Latitude"/>
+    <tableColumn id="7" xr3:uid="{38234185-885C-417C-BEC6-8B0AAC5BC3AF}" name="Shelter Latitude"/>
+    <tableColumn id="8" xr3:uid="{2914792C-C302-4F22-9934-AAC0281D3D53}" name="Shelter Longitude"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,65 +1106,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1196,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1223,28 +1223,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,43 +1765,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed report template, optimized routing
report preview now works
</commit_message>
<xml_diff>
--- a/ProgramSrc/ReportTemplate.xlsx
+++ b/ProgramSrc/ReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\ProgramSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah\Documents\GitHub Repositories\ShelterAlloc_Thesis\ProgramSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D2987-C7F1-457D-A7A2-062BA3E6AFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEECB02C-E0B6-4146-ADB9-77498C941245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{EDF13D95-9A8A-4EF7-9253-EE93AC25A225}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{EDF13D95-9A8A-4EF7-9253-EE93AC25A225}"/>
   </bookViews>
   <sheets>
     <sheet name="Shelter Location-Allocation" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>xDegrees</t>
-  </si>
-  <si>
-    <t>yDegrees</t>
-  </si>
-  <si>
     <t>Area1</t>
   </si>
   <si>
@@ -121,6 +115,12 @@
   </si>
   <si>
     <t>Allocated Population</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -759,8 +759,8 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1098318C-F159-4C06-B902-D5D443D7C297}" name="Active" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D82E8B3A-327A-4383-95EC-C438C730630C}" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{94A21AA9-4F96-42F9-8A64-37BF1E4A18FC}" name="xDegrees" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3BE3E6B1-E055-463F-A06B-0316E0AF650B}" name="yDegrees" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{94A21AA9-4F96-42F9-8A64-37BF1E4A18FC}" name="Latitude" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3BE3E6B1-E055-463F-A06B-0316E0AF650B}" name="Longitude" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{45060683-C166-4811-833F-3CC9CFE3CD05}" name="Population" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{B7B71B5A-E127-4E4E-983E-C67B9AF1ECDF}" name="AffectedPop" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{79FBC0B9-2EEB-4387-A81C-B2877E002D78}" name="MaxDistance" dataDxfId="1"/>
@@ -776,8 +776,8 @@
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{013C82DD-DF1C-49FE-9CF4-1AD7939141F3}" name="Active"/>
     <tableColumn id="2" xr3:uid="{8B704143-D213-4B0B-9C69-618BAB6CAA83}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{0CFA250A-AC5B-4CFE-A2BE-B2792DA4C149}" name="xDegrees"/>
-    <tableColumn id="4" xr3:uid="{078AE196-143A-4E3C-A4DA-9863CC58CDDB}" name="yDegrees"/>
+    <tableColumn id="3" xr3:uid="{0CFA250A-AC5B-4CFE-A2BE-B2792DA4C149}" name="Latitude"/>
+    <tableColumn id="4" xr3:uid="{078AE196-143A-4E3C-A4DA-9863CC58CDDB}" name="Longitude"/>
     <tableColumn id="5" xr3:uid="{FAA9629F-56B6-4022-A286-AAD99C8DE3B3}" name="Area1"/>
     <tableColumn id="6" xr3:uid="{586289DE-F915-40D9-BC55-9F5E99D1A346}" name="Cost1"/>
     <tableColumn id="7" xr3:uid="{D45A5453-8E8F-4A8A-9288-F90210D4DF63}" name="Area2"/>
@@ -793,9 +793,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -833,7 +833,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -939,7 +939,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1081,7 +1081,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1091,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A918FFA0-D07D-44CC-B35F-E2BA18996B1D}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1146,25 +1146,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1212,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,22 +1229,22 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F6E060-A238-4890-9731-8C688E2E947F}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,37 +1771,37 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>